<commit_message>
further improve argument validation and testing
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/time_series_invalid_sheet.xlsx
+++ b/tests/testthat/fixtures/time_series_invalid_sheet.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gleb/polybox/PhD/Science/Software/tecanr/tests/testthat/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AB9AFB-3625-6040-AED3-6294C67177BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76AF087-E983-234C-A56F-40A3F9CFFE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="500" windowWidth="14940" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="invalid sheet" sheetId="5" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -33,7 +33,7 @@
     <author>Lab User</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F14FC6C6-A9A1-814A-A312-AB13CC1A3284}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{2AEC0222-9E06-AE4F-9F8F-2B19B5F1A1F0}">
       <text>
         <r>
           <rPr>
@@ -598,7 +598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{9E4392E7-9721-3F45-B52E-316962165F01}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{12CD0B66-779A-484A-9430-B30493E6CBE4}">
       <text>
         <r>
           <rPr>
@@ -628,6 +628,601 @@
     <author>Lab User</author>
   </authors>
   <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F14FC6C6-A9A1-814A-A312-AB13CC1A3284}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common.DocumentManagement, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common.DocumentManagement.Reader, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common.MCS, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common.Results, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common.UI, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.Common, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.Port.IP, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.Port.RS232, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.Port.SIM.Common, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.Port.USB, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.Server, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.AMR, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.AMRPlus, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.Connect, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.GeniosUltra, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.Safire3, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.Safire3Pro, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Communication.SIM.SunriseMini, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Common, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Common.GCM, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Common.Reader, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Common.Stacker, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Gas.GCM, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.GCM.Server, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Reader.AMR, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Reader.AMRPlus, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Reader.GeniosUltra, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Reader.Safire3, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Reader.Safire3Pro, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Reader.SunriseMini, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Server, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Stacker.Connect, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Instrument.Stacker.Server, 3.9.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Measurement.BuiltInTest.Common, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Measurement.Common, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Measurement.Server, 3.6.1.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Connect.Reader, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Core, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.AMR, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.AMRPlus, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.GeniosUltra, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.Reader, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.Safire3, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.Safire3Pro, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.Device.SunriseMini, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.ExcelOutput, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.NanoQuant, 2.0.10.0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.XFluor.ReaderEditor, 2.0.10.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{9E4392E7-9721-3F45-B52E-316962165F01}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">EHC, V_3.40_01/15_Infinite (Dec 23 2014/12.45.11)
+MTP, V_3.40_01/15_Infinite (Dec 23 2014/12.45.11)
+HCP, V_2.02_05/06_HCP (May 23 2006/14.05.27)
+MEM, V_3.00_09/11_MCR (Sep 27 2011/15.05.45)
+MEX, V_3.00_09/11_MCR (Sep 27 2011/15.05.10)
+ZSCAN, V_3.40_01/15_Infinite (Dec 23 2014/12.45.11)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lab User</author>
+  </authors>
+  <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
@@ -1218,7 +1813,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="65">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -1413,9 +2008,6 @@
   </si>
   <si>
     <t>1/1/2022 12:00:00 PM</t>
-  </si>
-  <si>
-    <t>this sheet is not empty, but there is also no data here</t>
   </si>
 </sst>
 </file>
@@ -1714,6 +2306,256 @@
           <c:bubble3D val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C21-C546-914C-1CE8E89D5CF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:bubbleSize>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4C21-C546-914C-1CE8E89D5CF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="50"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="2024529695"/>
+        <c:axId val="2024535103"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="2024529695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2024535103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2024535103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2024529695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Multiple Reads Per Well - Alignment</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5B9BD5"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr sz="800"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-CH"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>0</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5D83-C640-854D-4B2859C51BC9}"/>
             </c:ext>
           </c:extLst>
@@ -1818,7 +2660,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -2074,6 +2916,49 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="_chart_1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28C9136-B942-CE4D-A845-B6A6861747CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
@@ -2111,7 +2996,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2414,22 +3299,2453 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C6D9F0-EEB3-9B4A-9366-1E521A912D77}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D66A6-44A8-2342-B2BD-E70D42866FC9}">
+  <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.13194444444444445</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>1500</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27">
+        <v>600</v>
+      </c>
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5">
+        <v>2</v>
+      </c>
+      <c r="D54" s="5">
+        <v>3</v>
+      </c>
+      <c r="E54" s="5">
+        <v>4</v>
+      </c>
+      <c r="F54" s="5">
+        <v>5</v>
+      </c>
+      <c r="G54" s="5">
+        <v>6</v>
+      </c>
+      <c r="H54" s="5">
+        <v>7</v>
+      </c>
+      <c r="I54" s="5">
+        <v>8</v>
+      </c>
+      <c r="J54" s="5">
+        <v>9</v>
+      </c>
+      <c r="K54" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>600</v>
+      </c>
+      <c r="D55">
+        <v>1200</v>
+      </c>
+      <c r="E55">
+        <v>1800</v>
+      </c>
+      <c r="F55">
+        <v>2400</v>
+      </c>
+      <c r="G55">
+        <v>3000</v>
+      </c>
+      <c r="H55">
+        <v>3600</v>
+      </c>
+      <c r="I55">
+        <v>4200</v>
+      </c>
+      <c r="J55">
+        <v>4800</v>
+      </c>
+      <c r="K55">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56">
+        <v>30.8</v>
+      </c>
+      <c r="C56">
+        <v>30.8</v>
+      </c>
+      <c r="D56">
+        <v>31</v>
+      </c>
+      <c r="E56">
+        <v>30.9</v>
+      </c>
+      <c r="F56">
+        <v>30.9</v>
+      </c>
+      <c r="G56">
+        <v>31.2</v>
+      </c>
+      <c r="H56">
+        <v>31.2</v>
+      </c>
+      <c r="I56">
+        <v>31.3</v>
+      </c>
+      <c r="J56">
+        <v>31</v>
+      </c>
+      <c r="K56">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="C57">
+        <v>9.960000216960907E-2</v>
+      </c>
+      <c r="D57">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="E57">
+        <v>9.9799998104572296E-2</v>
+      </c>
+      <c r="F57">
+        <v>9.960000216960907E-2</v>
+      </c>
+      <c r="G57">
+        <v>9.9899999797344208E-2</v>
+      </c>
+      <c r="H57">
+        <v>9.920000284910202E-2</v>
+      </c>
+      <c r="I57">
+        <v>9.8999999463558197E-2</v>
+      </c>
+      <c r="J57">
+        <v>9.9299997091293335E-2</v>
+      </c>
+      <c r="K57">
+        <v>9.8200000822544098E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58">
+        <v>1.7599999904632568E-2</v>
+      </c>
+      <c r="C58">
+        <v>1.5699999406933784E-2</v>
+      </c>
+      <c r="D58">
+        <v>1.6899999231100082E-2</v>
+      </c>
+      <c r="E58">
+        <v>1.6499999910593033E-2</v>
+      </c>
+      <c r="F58">
+        <v>1.5599999576807022E-2</v>
+      </c>
+      <c r="G58">
+        <v>1.5799999237060547E-2</v>
+      </c>
+      <c r="H58">
+        <v>1.4700000174343586E-2</v>
+      </c>
+      <c r="I58">
+        <v>1.4499999582767487E-2</v>
+      </c>
+      <c r="J58">
+        <v>1.5599999576807022E-2</v>
+      </c>
+      <c r="K58">
+        <v>1.3700000010430813E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59">
+        <v>9.2200003564357758E-2</v>
+      </c>
+      <c r="C59">
+        <v>9.2000000178813934E-2</v>
+      </c>
+      <c r="D59">
+        <v>9.2100001871585846E-2</v>
+      </c>
+      <c r="E59">
+        <v>9.1700002551078796E-2</v>
+      </c>
+      <c r="F59">
+        <v>9.1600000858306885E-2</v>
+      </c>
+      <c r="G59">
+        <v>9.1700002551078796E-2</v>
+      </c>
+      <c r="H59">
+        <v>9.1499999165534973E-2</v>
+      </c>
+      <c r="I59">
+        <v>9.2000000178813934E-2</v>
+      </c>
+      <c r="J59">
+        <v>9.1799996793270111E-2</v>
+      </c>
+      <c r="K59">
+        <v>9.1399997472763062E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60">
+        <v>0.13179999589920044</v>
+      </c>
+      <c r="C60">
+        <v>0.12700000405311584</v>
+      </c>
+      <c r="D60">
+        <v>0.12980000674724579</v>
+      </c>
+      <c r="E60">
+        <v>0.12890000641345978</v>
+      </c>
+      <c r="F60">
+        <v>0.12710000574588776</v>
+      </c>
+      <c r="G60">
+        <v>0.12749999761581421</v>
+      </c>
+      <c r="H60">
+        <v>0.125</v>
+      </c>
+      <c r="I60">
+        <v>0.12430000305175781</v>
+      </c>
+      <c r="J60">
+        <v>0.12680000066757202</v>
+      </c>
+      <c r="K60">
+        <v>0.12229999899864197</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61">
+        <v>8.8899999856948853E-2</v>
+      </c>
+      <c r="C61">
+        <v>8.8799998164176941E-2</v>
+      </c>
+      <c r="D61">
+        <v>8.8399998843669891E-2</v>
+      </c>
+      <c r="E61">
+        <v>8.9000001549720764E-2</v>
+      </c>
+      <c r="F61">
+        <v>8.8899999856948853E-2</v>
+      </c>
+      <c r="G61">
+        <v>8.919999748468399E-2</v>
+      </c>
+      <c r="H61">
+        <v>8.9400000870227814E-2</v>
+      </c>
+      <c r="I61">
+        <v>8.9000001549720764E-2</v>
+      </c>
+      <c r="J61">
+        <v>9.0099997818470001E-2</v>
+      </c>
+      <c r="K61">
+        <v>8.9900001883506775E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62">
+        <v>9.8399996757507324E-2</v>
+      </c>
+      <c r="C62">
+        <v>9.790000319480896E-2</v>
+      </c>
+      <c r="D62">
+        <v>9.7000002861022949E-2</v>
+      </c>
+      <c r="E62">
+        <v>9.7000002861022949E-2</v>
+      </c>
+      <c r="F62">
+        <v>9.7300000488758087E-2</v>
+      </c>
+      <c r="G62">
+        <v>9.8099999129772186E-2</v>
+      </c>
+      <c r="H62">
+        <v>9.7599998116493225E-2</v>
+      </c>
+      <c r="I62">
+        <v>9.7599998116493225E-2</v>
+      </c>
+      <c r="J62">
+        <v>9.5799997448921204E-2</v>
+      </c>
+      <c r="K62">
+        <v>9.6000000834465027E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63">
+        <v>9.3199998140335083E-2</v>
+      </c>
+      <c r="C63">
+        <v>9.2299997806549072E-2</v>
+      </c>
+      <c r="D63">
+        <v>9.2900000512599945E-2</v>
+      </c>
+      <c r="E63">
+        <v>9.2600002884864807E-2</v>
+      </c>
+      <c r="F63">
+        <v>9.3199998140335083E-2</v>
+      </c>
+      <c r="G63">
+        <v>9.2799998819828033E-2</v>
+      </c>
+      <c r="H63">
+        <v>9.2600002884864807E-2</v>
+      </c>
+      <c r="I63">
+        <v>9.2000000178813934E-2</v>
+      </c>
+      <c r="J63">
+        <v>9.1799996793270111E-2</v>
+      </c>
+      <c r="K63">
+        <v>9.1399997472763062E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" s="5">
+        <v>1</v>
+      </c>
+      <c r="C66" s="5">
+        <v>2</v>
+      </c>
+      <c r="D66" s="5">
+        <v>3</v>
+      </c>
+      <c r="E66" s="5">
+        <v>4</v>
+      </c>
+      <c r="F66" s="5">
+        <v>5</v>
+      </c>
+      <c r="G66" s="5">
+        <v>6</v>
+      </c>
+      <c r="H66" s="5">
+        <v>7</v>
+      </c>
+      <c r="I66" s="5">
+        <v>8</v>
+      </c>
+      <c r="J66" s="5">
+        <v>9</v>
+      </c>
+      <c r="K66" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>600</v>
+      </c>
+      <c r="D67">
+        <v>1200</v>
+      </c>
+      <c r="E67">
+        <v>1800</v>
+      </c>
+      <c r="F67">
+        <v>2400</v>
+      </c>
+      <c r="G67">
+        <v>3000</v>
+      </c>
+      <c r="H67">
+        <v>3600</v>
+      </c>
+      <c r="I67">
+        <v>4200</v>
+      </c>
+      <c r="J67">
+        <v>4800</v>
+      </c>
+      <c r="K67">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68">
+        <v>30.8</v>
+      </c>
+      <c r="C68">
+        <v>30.8</v>
+      </c>
+      <c r="D68">
+        <v>31</v>
+      </c>
+      <c r="E68">
+        <v>30.9</v>
+      </c>
+      <c r="F68">
+        <v>30.9</v>
+      </c>
+      <c r="G68">
+        <v>31.2</v>
+      </c>
+      <c r="H68">
+        <v>31.2</v>
+      </c>
+      <c r="I68">
+        <v>31.3</v>
+      </c>
+      <c r="J68">
+        <v>31</v>
+      </c>
+      <c r="K68">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69">
+        <v>0.10300000011920929</v>
+      </c>
+      <c r="C69">
+        <v>0.10189999639987946</v>
+      </c>
+      <c r="D69">
+        <v>0.10189999639987946</v>
+      </c>
+      <c r="E69">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="F69">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="G69">
+        <v>9.8800003528594971E-2</v>
+      </c>
+      <c r="H69">
+        <v>0.10050000250339508</v>
+      </c>
+      <c r="I69">
+        <v>0.10029999911785126</v>
+      </c>
+      <c r="J69">
+        <v>0.10010000318288803</v>
+      </c>
+      <c r="K69">
+        <v>9.9299997091293335E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70">
+        <v>1.510000042617321E-2</v>
+      </c>
+      <c r="C70">
+        <v>1.4200000092387199E-2</v>
+      </c>
+      <c r="D70">
+        <v>1.4600000344216824E-2</v>
+      </c>
+      <c r="E70">
+        <v>1.4100000262260437E-2</v>
+      </c>
+      <c r="F70">
+        <v>1.4399999752640724E-2</v>
+      </c>
+      <c r="G70">
+        <v>1.2600000016391277E-2</v>
+      </c>
+      <c r="H70">
+        <v>1.4499999582767487E-2</v>
+      </c>
+      <c r="I70">
+        <v>1.3899999670684338E-2</v>
+      </c>
+      <c r="J70">
+        <v>1.3500000350177288E-2</v>
+      </c>
+      <c r="K70">
+        <v>1.2799999676644802E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B71">
+        <v>9.4400003552436829E-2</v>
+      </c>
+      <c r="C71">
+        <v>9.3800000846385956E-2</v>
+      </c>
+      <c r="D71">
+        <v>9.4200000166893005E-2</v>
+      </c>
+      <c r="E71">
+        <v>9.3500003218650818E-2</v>
+      </c>
+      <c r="F71">
+        <v>9.3000002205371857E-2</v>
+      </c>
+      <c r="G71">
+        <v>9.3800000846385956E-2</v>
+      </c>
+      <c r="H71">
+        <v>9.3500003218650818E-2</v>
+      </c>
+      <c r="I71">
+        <v>9.3599997460842133E-2</v>
+      </c>
+      <c r="J71">
+        <v>9.4700001180171967E-2</v>
+      </c>
+      <c r="K71">
+        <v>9.3299999833106995E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72">
+        <v>0.12590000033378601</v>
+      </c>
+      <c r="C72">
+        <v>0.12409999966621399</v>
+      </c>
+      <c r="D72">
+        <v>0.12590000033378601</v>
+      </c>
+      <c r="E72">
+        <v>0.12430000305175781</v>
+      </c>
+      <c r="F72">
+        <v>0.12460000067949295</v>
+      </c>
+      <c r="G72">
+        <v>0.12020000070333481</v>
+      </c>
+      <c r="H72">
+        <v>0.12489999830722809</v>
+      </c>
+      <c r="I72">
+        <v>0.12380000203847885</v>
+      </c>
+      <c r="J72">
+        <v>0.12330000102519989</v>
+      </c>
+      <c r="K72">
+        <v>0.12099999934434891</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73">
+        <v>8.959999680519104E-2</v>
+      </c>
+      <c r="C73">
+        <v>8.9500002562999725E-2</v>
+      </c>
+      <c r="D73">
+        <v>8.9000001549720764E-2</v>
+      </c>
+      <c r="E73">
+        <v>8.959999680519104E-2</v>
+      </c>
+      <c r="F73">
+        <v>8.9100003242492676E-2</v>
+      </c>
+      <c r="G73">
+        <v>8.829999715089798E-2</v>
+      </c>
+      <c r="H73">
+        <v>8.8699996471405029E-2</v>
+      </c>
+      <c r="I73">
+        <v>8.9500002562999725E-2</v>
+      </c>
+      <c r="J73">
+        <v>8.8799998164176941E-2</v>
+      </c>
+      <c r="K73">
+        <v>8.9100003242492676E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74">
+        <v>0.11060000211000443</v>
+      </c>
+      <c r="C74">
+        <v>0.10790000110864639</v>
+      </c>
+      <c r="D74">
+        <v>0.10509999841451645</v>
+      </c>
+      <c r="E74">
+        <v>0.10429999977350235</v>
+      </c>
+      <c r="F74">
+        <v>0.1039000004529953</v>
+      </c>
+      <c r="G74">
+        <v>9.8800003528594971E-2</v>
+      </c>
+      <c r="H74">
+        <v>0.10220000147819519</v>
+      </c>
+      <c r="I74">
+        <v>0.10189999639987946</v>
+      </c>
+      <c r="J74">
+        <v>0.10019999742507935</v>
+      </c>
+      <c r="K74">
+        <v>0.1005999967455864</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75">
+        <v>9.4400003552436829E-2</v>
+      </c>
+      <c r="C75">
+        <v>9.3999996781349182E-2</v>
+      </c>
+      <c r="D75">
+        <v>9.5200002193450928E-2</v>
+      </c>
+      <c r="E75">
+        <v>9.3099996447563171E-2</v>
+      </c>
+      <c r="F75">
+        <v>9.3900002539157867E-2</v>
+      </c>
+      <c r="G75">
+        <v>9.2699997127056122E-2</v>
+      </c>
+      <c r="H75">
+        <v>9.3400001525878906E-2</v>
+      </c>
+      <c r="I75">
+        <v>9.2900000512599945E-2</v>
+      </c>
+      <c r="J75">
+        <v>9.3699999153614044E-2</v>
+      </c>
+      <c r="K75">
+        <v>9.2299997806549072E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" s="5">
+        <v>1</v>
+      </c>
+      <c r="C78" s="5">
+        <v>2</v>
+      </c>
+      <c r="D78" s="5">
+        <v>3</v>
+      </c>
+      <c r="E78" s="5">
+        <v>4</v>
+      </c>
+      <c r="F78" s="5">
+        <v>5</v>
+      </c>
+      <c r="G78" s="5">
+        <v>6</v>
+      </c>
+      <c r="H78" s="5">
+        <v>7</v>
+      </c>
+      <c r="I78" s="5">
+        <v>8</v>
+      </c>
+      <c r="J78" s="5">
+        <v>9</v>
+      </c>
+      <c r="K78" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>600</v>
+      </c>
+      <c r="D79">
+        <v>1200</v>
+      </c>
+      <c r="E79">
+        <v>1800</v>
+      </c>
+      <c r="F79">
+        <v>2400</v>
+      </c>
+      <c r="G79">
+        <v>3000</v>
+      </c>
+      <c r="H79">
+        <v>3600</v>
+      </c>
+      <c r="I79">
+        <v>4200</v>
+      </c>
+      <c r="J79">
+        <v>4800</v>
+      </c>
+      <c r="K79">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80">
+        <v>30.8</v>
+      </c>
+      <c r="C80">
+        <v>30.8</v>
+      </c>
+      <c r="D80">
+        <v>31</v>
+      </c>
+      <c r="E80">
+        <v>30.9</v>
+      </c>
+      <c r="F80">
+        <v>30.9</v>
+      </c>
+      <c r="G80">
+        <v>31.2</v>
+      </c>
+      <c r="H80">
+        <v>31.2</v>
+      </c>
+      <c r="I80">
+        <v>31.3</v>
+      </c>
+      <c r="J80">
+        <v>31</v>
+      </c>
+      <c r="K80">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81">
+        <v>0.10199999809265137</v>
+      </c>
+      <c r="C81">
+        <v>0.10109999775886536</v>
+      </c>
+      <c r="D81">
+        <v>0.10329999774694443</v>
+      </c>
+      <c r="E81">
+        <v>0.10520000010728836</v>
+      </c>
+      <c r="F81">
+        <v>0.10769999772310257</v>
+      </c>
+      <c r="G81">
+        <v>0.1080000028014183</v>
+      </c>
+      <c r="H81">
+        <v>0.10480000078678131</v>
+      </c>
+      <c r="I81">
+        <v>0.10369999706745148</v>
+      </c>
+      <c r="J81">
+        <v>0.10339999943971634</v>
+      </c>
+      <c r="K81">
+        <v>0.10149999707937241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82">
+        <v>1.5300000086426735E-2</v>
+      </c>
+      <c r="C82">
+        <v>1.4499999582767487E-2</v>
+      </c>
+      <c r="D82">
+        <v>1.3799999840557575E-2</v>
+      </c>
+      <c r="E82">
+        <v>1.4399999752640724E-2</v>
+      </c>
+      <c r="F82">
+        <v>1.510000042617321E-2</v>
+      </c>
+      <c r="G82">
+        <v>1.7999999225139618E-2</v>
+      </c>
+      <c r="H82">
+        <v>1.549999974668026E-2</v>
+      </c>
+      <c r="I82">
+        <v>1.5799999237060547E-2</v>
+      </c>
+      <c r="J82">
+        <v>1.5599999576807022E-2</v>
+      </c>
+      <c r="K82">
+        <v>1.4499999582767487E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83">
+        <v>0.10369999706745148</v>
+      </c>
+      <c r="C83">
+        <v>0.10170000046491623</v>
+      </c>
+      <c r="D83">
+        <v>0.10440000146627426</v>
+      </c>
+      <c r="E83">
+        <v>0.1023000031709671</v>
+      </c>
+      <c r="F83">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="G83">
+        <v>0.10260000079870224</v>
+      </c>
+      <c r="H83">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="I83">
+        <v>9.8600000143051147E-2</v>
+      </c>
+      <c r="J83">
+        <v>9.9500000476837158E-2</v>
+      </c>
+      <c r="K83">
+        <v>9.7099997103214264E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84">
+        <v>0.12759999930858612</v>
+      </c>
+      <c r="C84">
+        <v>0.12569999694824219</v>
+      </c>
+      <c r="D84">
+        <v>0.12669999897480011</v>
+      </c>
+      <c r="E84">
+        <v>0.13050000369548798</v>
+      </c>
+      <c r="F84">
+        <v>0.13249999284744263</v>
+      </c>
+      <c r="G84">
+        <v>0.1363999992609024</v>
+      </c>
+      <c r="H84">
+        <v>0.12960000336170197</v>
+      </c>
+      <c r="I84">
+        <v>0.13060000538825989</v>
+      </c>
+      <c r="J84">
+        <v>0.12989999353885651</v>
+      </c>
+      <c r="K84">
+        <v>0.1265999972820282</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B85">
+        <v>8.9000001549720764E-2</v>
+      </c>
+      <c r="C85">
+        <v>8.8899999856948853E-2</v>
+      </c>
+      <c r="D85">
+        <v>9.2799998819828033E-2</v>
+      </c>
+      <c r="E85">
+        <v>9.790000319480896E-2</v>
+      </c>
+      <c r="F85">
+        <v>9.9399998784065247E-2</v>
+      </c>
+      <c r="G85">
+        <v>9.2299997806549072E-2</v>
+      </c>
+      <c r="H85">
+        <v>9.1799996793270111E-2</v>
+      </c>
+      <c r="I85">
+        <v>9.1300003230571747E-2</v>
+      </c>
+      <c r="J85">
+        <v>9.1600000858306885E-2</v>
+      </c>
+      <c r="K85">
+        <v>9.0599998831748962E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B86">
+        <v>9.6199996769428253E-2</v>
+      </c>
+      <c r="C86">
+        <v>9.6199996769428253E-2</v>
+      </c>
+      <c r="D86">
+        <v>9.8499998450279236E-2</v>
+      </c>
+      <c r="E86">
+        <v>0.10109999775886536</v>
+      </c>
+      <c r="F86">
+        <v>0.11140000075101852</v>
+      </c>
+      <c r="G86">
+        <v>0.11429999768733978</v>
+      </c>
+      <c r="H86">
+        <v>0.10899999737739563</v>
+      </c>
+      <c r="I86">
+        <v>0.10429999977350235</v>
+      </c>
+      <c r="J86">
+        <v>0.10339999943971634</v>
+      </c>
+      <c r="K86">
+        <v>9.9799998104572296E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87">
+        <v>9.3800000846385956E-2</v>
+      </c>
+      <c r="C87">
+        <v>9.3199998140335083E-2</v>
+      </c>
+      <c r="D87">
+        <v>9.4200000166893005E-2</v>
+      </c>
+      <c r="E87">
+        <v>9.4499997794628143E-2</v>
+      </c>
+      <c r="F87">
+        <v>9.5100000500679016E-2</v>
+      </c>
+      <c r="G87">
+        <v>9.4499997794628143E-2</v>
+      </c>
+      <c r="H87">
+        <v>9.2600002884864807E-2</v>
+      </c>
+      <c r="I87">
+        <v>9.3800000846385956E-2</v>
+      </c>
+      <c r="J87">
+        <v>9.2600002884864807E-2</v>
+      </c>
+      <c r="K87">
+        <v>9.3400001525878906E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="5">
+        <v>1</v>
+      </c>
+      <c r="C90" s="5">
+        <v>2</v>
+      </c>
+      <c r="D90" s="5">
+        <v>3</v>
+      </c>
+      <c r="E90" s="5">
+        <v>4</v>
+      </c>
+      <c r="F90" s="5">
+        <v>5</v>
+      </c>
+      <c r="G90" s="5">
+        <v>6</v>
+      </c>
+      <c r="H90" s="5">
+        <v>7</v>
+      </c>
+      <c r="I90" s="5">
+        <v>8</v>
+      </c>
+      <c r="J90" s="5">
+        <v>9</v>
+      </c>
+      <c r="K90" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>600</v>
+      </c>
+      <c r="D91">
+        <v>1200</v>
+      </c>
+      <c r="E91">
+        <v>1800</v>
+      </c>
+      <c r="F91">
+        <v>2400</v>
+      </c>
+      <c r="G91">
+        <v>3000</v>
+      </c>
+      <c r="H91">
+        <v>3600</v>
+      </c>
+      <c r="I91">
+        <v>4200</v>
+      </c>
+      <c r="J91">
+        <v>4800</v>
+      </c>
+      <c r="K91">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92">
+        <v>30.8</v>
+      </c>
+      <c r="C92">
+        <v>30.8</v>
+      </c>
+      <c r="D92">
+        <v>31</v>
+      </c>
+      <c r="E92">
+        <v>30.9</v>
+      </c>
+      <c r="F92">
+        <v>30.9</v>
+      </c>
+      <c r="G92">
+        <v>31.2</v>
+      </c>
+      <c r="H92">
+        <v>31.2</v>
+      </c>
+      <c r="I92">
+        <v>31.3</v>
+      </c>
+      <c r="J92">
+        <v>31</v>
+      </c>
+      <c r="K92">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93">
+        <v>0.10419999808073044</v>
+      </c>
+      <c r="C93">
+        <v>0.1054999977350235</v>
+      </c>
+      <c r="D93">
+        <v>0.10459999740123749</v>
+      </c>
+      <c r="E93">
+        <v>0.10199999809265137</v>
+      </c>
+      <c r="F93">
+        <v>0.10170000046491623</v>
+      </c>
+      <c r="G93">
+        <v>0.10119999945163727</v>
+      </c>
+      <c r="H93">
+        <v>0.1005999967455864</v>
+      </c>
+      <c r="I93">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="J93">
+        <v>0.10019999742507935</v>
+      </c>
+      <c r="K93">
+        <v>9.8999999463558197E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B94">
+        <v>1.0700000450015068E-2</v>
+      </c>
+      <c r="C94">
+        <v>1.1900000274181366E-2</v>
+      </c>
+      <c r="D94">
+        <v>1.4700000174343586E-2</v>
+      </c>
+      <c r="E94">
+        <v>1.360000018030405E-2</v>
+      </c>
+      <c r="F94">
+        <v>1.2799999676644802E-2</v>
+      </c>
+      <c r="G94">
+        <v>1.3100000098347664E-2</v>
+      </c>
+      <c r="H94">
+        <v>1.3299999758601189E-2</v>
+      </c>
+      <c r="I94">
+        <v>1.2099999934434891E-2</v>
+      </c>
+      <c r="J94">
+        <v>1.1699999682605267E-2</v>
+      </c>
+      <c r="K94">
+        <v>1.119999960064888E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95">
+        <v>9.6400000154972076E-2</v>
+      </c>
+      <c r="C95">
+        <v>9.4300001859664917E-2</v>
+      </c>
+      <c r="D95">
+        <v>9.5299996435642242E-2</v>
+      </c>
+      <c r="E95">
+        <v>9.5100000500679016E-2</v>
+      </c>
+      <c r="F95">
+        <v>9.5200002193450928E-2</v>
+      </c>
+      <c r="G95">
+        <v>9.4599999487400055E-2</v>
+      </c>
+      <c r="H95">
+        <v>9.4300001859664917E-2</v>
+      </c>
+      <c r="I95">
+        <v>9.3999996781349182E-2</v>
+      </c>
+      <c r="J95">
+        <v>9.4999998807907104E-2</v>
+      </c>
+      <c r="K95">
+        <v>9.3800000846385956E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96">
+        <v>0.11919999867677689</v>
+      </c>
+      <c r="C96">
+        <v>0.12160000205039978</v>
+      </c>
+      <c r="D96">
+        <v>0.12319999933242798</v>
+      </c>
+      <c r="E96">
+        <v>0.12200000137090683</v>
+      </c>
+      <c r="F96">
+        <v>0.12060000002384186</v>
+      </c>
+      <c r="G96">
+        <v>0.12039999663829803</v>
+      </c>
+      <c r="H96">
+        <v>0.12030000239610672</v>
+      </c>
+      <c r="I96">
+        <v>0.11800000071525574</v>
+      </c>
+      <c r="J96">
+        <v>0.11699999868869781</v>
+      </c>
+      <c r="K96">
+        <v>0.11580000072717667</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B97">
+        <v>0.11020000278949738</v>
+      </c>
+      <c r="C97">
+        <v>0.1096000000834465</v>
+      </c>
+      <c r="D97">
+        <v>9.3699999153614044E-2</v>
+      </c>
+      <c r="E97">
+        <v>9.0400002896785736E-2</v>
+      </c>
+      <c r="F97">
+        <v>9.0300001204013824E-2</v>
+      </c>
+      <c r="G97">
+        <v>8.9800000190734863E-2</v>
+      </c>
+      <c r="H97">
+        <v>8.9400000870227814E-2</v>
+      </c>
+      <c r="I97">
+        <v>8.9900001883506775E-2</v>
+      </c>
+      <c r="J97">
+        <v>9.0199999511241913E-2</v>
+      </c>
+      <c r="K97">
+        <v>8.959999680519104E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B98">
+        <v>0.10249999910593033</v>
+      </c>
+      <c r="C98">
+        <v>0.10899999737739563</v>
+      </c>
+      <c r="D98">
+        <v>0.11779999732971191</v>
+      </c>
+      <c r="E98">
+        <v>0.11020000278949738</v>
+      </c>
+      <c r="F98">
+        <v>0.10920000076293945</v>
+      </c>
+      <c r="G98">
+        <v>0.10899999737739563</v>
+      </c>
+      <c r="H98">
+        <v>0.10819999873638153</v>
+      </c>
+      <c r="I98">
+        <v>0.10700000077486038</v>
+      </c>
+      <c r="J98">
+        <v>0.10779999941587448</v>
+      </c>
+      <c r="K98">
+        <v>0.10499999672174454</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B99">
+        <v>9.2799998819828033E-2</v>
+      </c>
+      <c r="C99">
+        <v>9.3099996447563171E-2</v>
+      </c>
+      <c r="D99">
+        <v>9.3000002205371857E-2</v>
+      </c>
+      <c r="E99">
+        <v>9.2200003564357758E-2</v>
+      </c>
+      <c r="F99">
+        <v>9.3299999833106995E-2</v>
+      </c>
+      <c r="G99">
+        <v>9.2000000178813934E-2</v>
+      </c>
+      <c r="H99">
+        <v>9.0800002217292786E-2</v>
+      </c>
+      <c r="I99">
+        <v>9.1300003230571747E-2</v>
+      </c>
+      <c r="J99">
+        <v>9.1200001537799835E-2</v>
+      </c>
+      <c r="K99">
+        <v>9.0700000524520874E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B102" s="5">
+        <v>1</v>
+      </c>
+      <c r="C102" s="5">
+        <v>2</v>
+      </c>
+      <c r="D102" s="5">
+        <v>3</v>
+      </c>
+      <c r="E102" s="5">
+        <v>4</v>
+      </c>
+      <c r="F102" s="5">
+        <v>5</v>
+      </c>
+      <c r="G102" s="5">
+        <v>6</v>
+      </c>
+      <c r="H102" s="5">
+        <v>7</v>
+      </c>
+      <c r="I102" s="5">
+        <v>8</v>
+      </c>
+      <c r="J102" s="5">
+        <v>9</v>
+      </c>
+      <c r="K102" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>600</v>
+      </c>
+      <c r="D103">
+        <v>1200</v>
+      </c>
+      <c r="E103">
+        <v>1800</v>
+      </c>
+      <c r="F103">
+        <v>2400</v>
+      </c>
+      <c r="G103">
+        <v>3000</v>
+      </c>
+      <c r="H103">
+        <v>3600</v>
+      </c>
+      <c r="I103">
+        <v>4200</v>
+      </c>
+      <c r="J103">
+        <v>4800</v>
+      </c>
+      <c r="K103">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104">
+        <v>30.8</v>
+      </c>
+      <c r="C104">
+        <v>30.8</v>
+      </c>
+      <c r="D104">
+        <v>31</v>
+      </c>
+      <c r="E104">
+        <v>30.9</v>
+      </c>
+      <c r="F104">
+        <v>30.9</v>
+      </c>
+      <c r="G104">
+        <v>31.2</v>
+      </c>
+      <c r="H104">
+        <v>31.2</v>
+      </c>
+      <c r="I104">
+        <v>31.3</v>
+      </c>
+      <c r="J104">
+        <v>31</v>
+      </c>
+      <c r="K104">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105">
+        <v>0.10440000146627426</v>
+      </c>
+      <c r="C105">
+        <v>0.10409999638795853</v>
+      </c>
+      <c r="D105">
+        <v>0.10350000113248825</v>
+      </c>
+      <c r="E105">
+        <v>0.10249999910593033</v>
+      </c>
+      <c r="F105">
+        <v>0.10409999638795853</v>
+      </c>
+      <c r="G105">
+        <v>0.10140000283718109</v>
+      </c>
+      <c r="H105">
+        <v>0.10239999741315842</v>
+      </c>
+      <c r="I105">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="J105">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="K105">
+        <v>0.10019999742507935</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106">
+        <v>1.549999974668026E-2</v>
+      </c>
+      <c r="C106">
+        <v>1.4700000174343586E-2</v>
+      </c>
+      <c r="D106">
+        <v>1.2900000438094139E-2</v>
+      </c>
+      <c r="E106">
+        <v>1.1900000274181366E-2</v>
+      </c>
+      <c r="F106">
+        <v>1.360000018030405E-2</v>
+      </c>
+      <c r="G106">
+        <v>1.0499999858438969E-2</v>
+      </c>
+      <c r="H106">
+        <v>1.0300000198185444E-2</v>
+      </c>
+      <c r="I106">
+        <v>8.2000000402331352E-3</v>
+      </c>
+      <c r="J106">
+        <v>7.3000001721084118E-3</v>
+      </c>
+      <c r="K106">
+        <v>7.4000000022351742E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107">
+        <v>0.10540000349283218</v>
+      </c>
+      <c r="C107">
+        <v>0.10440000146627426</v>
+      </c>
+      <c r="D107">
+        <v>0.1088000014424324</v>
+      </c>
+      <c r="E107">
+        <v>0.10289999842643738</v>
+      </c>
+      <c r="F107">
+        <v>0.10279999673366547</v>
+      </c>
+      <c r="G107">
+        <v>0.1054999977350235</v>
+      </c>
+      <c r="H107">
+        <v>0.10920000076293945</v>
+      </c>
+      <c r="I107">
+        <v>0.10360000282526016</v>
+      </c>
+      <c r="J107">
+        <v>0.10429999977350235</v>
+      </c>
+      <c r="K107">
+        <v>0.10559999942779541</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B108">
+        <v>0.12649999558925629</v>
+      </c>
+      <c r="C108">
+        <v>0.12129999697208405</v>
+      </c>
+      <c r="D108">
+        <v>0.11749999970197678</v>
+      </c>
+      <c r="E108">
+        <v>0.11450000107288361</v>
+      </c>
+      <c r="F108">
+        <v>0.11789999902248383</v>
+      </c>
+      <c r="G108">
+        <v>0.11429999768733978</v>
+      </c>
+      <c r="H108">
+        <v>0.11410000175237656</v>
+      </c>
+      <c r="I108">
+        <v>0.11240000277757645</v>
+      </c>
+      <c r="J108">
+        <v>0.10980000346899033</v>
+      </c>
+      <c r="K108">
+        <v>0.10909999907016754</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B109">
+        <v>8.8200002908706665E-2</v>
+      </c>
+      <c r="C109">
+        <v>8.8200002908706665E-2</v>
+      </c>
+      <c r="D109">
+        <v>8.829999715089798E-2</v>
+      </c>
+      <c r="E109">
+        <v>8.8500000536441803E-2</v>
+      </c>
+      <c r="F109">
+        <v>8.829999715089798E-2</v>
+      </c>
+      <c r="G109">
+        <v>8.8600002229213715E-2</v>
+      </c>
+      <c r="H109">
+        <v>8.8799998164176941E-2</v>
+      </c>
+      <c r="I109">
+        <v>9.0300001204013824E-2</v>
+      </c>
+      <c r="J109">
+        <v>9.0999998152256012E-2</v>
+      </c>
+      <c r="K109">
+        <v>9.0199999511241913E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B110">
+        <v>0.11069999635219574</v>
+      </c>
+      <c r="C110">
+        <v>0.11590000241994858</v>
+      </c>
+      <c r="D110">
+        <v>0.11159999668598175</v>
+      </c>
+      <c r="E110">
+        <v>0.11410000175237656</v>
+      </c>
+      <c r="F110">
+        <v>0.11779999732971191</v>
+      </c>
+      <c r="G110">
+        <v>0.10589999705553055</v>
+      </c>
+      <c r="H110">
+        <v>0.1046999990940094</v>
+      </c>
+      <c r="I110">
+        <v>0.10140000283718109</v>
+      </c>
+      <c r="J110">
+        <v>0.10289999842643738</v>
+      </c>
+      <c r="K110">
+        <v>9.8499998450279236E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B111">
+        <v>9.1399997472763062E-2</v>
+      </c>
+      <c r="C111">
+        <v>9.0700000524520874E-2</v>
+      </c>
+      <c r="D111">
+        <v>9.1399997472763062E-2</v>
+      </c>
+      <c r="E111">
+        <v>9.2699997127056122E-2</v>
+      </c>
+      <c r="F111">
+        <v>9.3599997460842133E-2</v>
+      </c>
+      <c r="G111">
+        <v>9.2600002884864807E-2</v>
+      </c>
+      <c r="H111">
+        <v>9.5100000500679016E-2</v>
+      </c>
+      <c r="I111">
+        <v>9.6900001168251038E-2</v>
+      </c>
+      <c r="J111">
+        <v>9.6199996769428253E-2</v>
+      </c>
+      <c r="K111">
+        <v>9.7499996423721313E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B114" s="5">
+        <v>1</v>
+      </c>
+      <c r="C114" s="5">
+        <v>2</v>
+      </c>
+      <c r="D114" s="5">
+        <v>3</v>
+      </c>
+      <c r="E114" s="5">
+        <v>4</v>
+      </c>
+      <c r="F114" s="5">
+        <v>5</v>
+      </c>
+      <c r="G114" s="5">
+        <v>6</v>
+      </c>
+      <c r="H114" s="5">
+        <v>7</v>
+      </c>
+      <c r="I114" s="5">
+        <v>8</v>
+      </c>
+      <c r="J114" s="5">
+        <v>9</v>
+      </c>
+      <c r="K114" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>600</v>
+      </c>
+      <c r="D115">
+        <v>1200</v>
+      </c>
+      <c r="E115">
+        <v>1800</v>
+      </c>
+      <c r="F115">
+        <v>2400</v>
+      </c>
+      <c r="G115">
+        <v>3000</v>
+      </c>
+      <c r="H115">
+        <v>3600</v>
+      </c>
+      <c r="I115">
+        <v>4200</v>
+      </c>
+      <c r="J115">
+        <v>4800</v>
+      </c>
+      <c r="K115">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B116">
+        <v>30.8</v>
+      </c>
+      <c r="C116">
+        <v>30.8</v>
+      </c>
+      <c r="D116">
+        <v>31</v>
+      </c>
+      <c r="E116">
+        <v>30.9</v>
+      </c>
+      <c r="F116">
+        <v>30.9</v>
+      </c>
+      <c r="G116">
+        <v>31.2</v>
+      </c>
+      <c r="H116">
+        <v>31.2</v>
+      </c>
+      <c r="I116">
+        <v>31.3</v>
+      </c>
+      <c r="J116">
+        <v>31</v>
+      </c>
+      <c r="K116">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B117">
+        <v>0.1039000004529953</v>
+      </c>
+      <c r="C117">
+        <v>0.10429999977350235</v>
+      </c>
+      <c r="D117">
+        <v>0.10450000315904617</v>
+      </c>
+      <c r="E117">
+        <v>0.10440000146627426</v>
+      </c>
+      <c r="F117">
+        <v>0.1046999990940094</v>
+      </c>
+      <c r="G117">
+        <v>0.10360000282526016</v>
+      </c>
+      <c r="H117">
+        <v>0.10300000011920929</v>
+      </c>
+      <c r="I117">
+        <v>0.10360000282526016</v>
+      </c>
+      <c r="J117">
+        <v>0.10320000350475311</v>
+      </c>
+      <c r="K117">
+        <v>0.10239999741315842</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B118">
+        <v>1.3500000350177288E-2</v>
+      </c>
+      <c r="C118">
+        <v>1.4200000092387199E-2</v>
+      </c>
+      <c r="D118">
+        <v>1.3799999840557575E-2</v>
+      </c>
+      <c r="E118">
+        <v>1.3799999840557575E-2</v>
+      </c>
+      <c r="F118">
+        <v>1.3899999670684338E-2</v>
+      </c>
+      <c r="G118">
+        <v>1.4000000432133675E-2</v>
+      </c>
+      <c r="H118">
+        <v>1.3299999758601189E-2</v>
+      </c>
+      <c r="I118">
+        <v>1.3899999670684338E-2</v>
+      </c>
+      <c r="J118">
+        <v>1.4100000262260437E-2</v>
+      </c>
+      <c r="K118">
+        <v>1.2799999676644802E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B119">
+        <v>9.9299997091293335E-2</v>
+      </c>
+      <c r="C119">
+        <v>0.10040000081062317</v>
+      </c>
+      <c r="D119">
+        <v>0.1031000018119812</v>
+      </c>
+      <c r="E119">
+        <v>0.10189999639987946</v>
+      </c>
+      <c r="F119">
+        <v>0.10329999774694443</v>
+      </c>
+      <c r="G119">
+        <v>0.10080000013113022</v>
+      </c>
+      <c r="H119">
+        <v>0.10130000114440918</v>
+      </c>
+      <c r="I119">
+        <v>0.10090000182390213</v>
+      </c>
+      <c r="J119">
+        <v>0.10069999843835831</v>
+      </c>
+      <c r="K119">
+        <v>0.10050000250339508</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B120">
+        <v>0.1128000020980835</v>
+      </c>
+      <c r="C120">
+        <v>0.11479999870061874</v>
+      </c>
+      <c r="D120">
+        <v>0.11270000040531158</v>
+      </c>
+      <c r="E120">
+        <v>0.11379999667406082</v>
+      </c>
+      <c r="F120">
+        <v>0.11270000040531158</v>
+      </c>
+      <c r="G120">
+        <v>0.11209999769926071</v>
+      </c>
+      <c r="H120">
+        <v>0.11020000278949738</v>
+      </c>
+      <c r="I120">
+        <v>0.11129999905824661</v>
+      </c>
+      <c r="J120">
+        <v>0.1096000000834465</v>
+      </c>
+      <c r="K120">
+        <v>0.10899999737739563</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B121">
+        <v>9.3699999153614044E-2</v>
+      </c>
+      <c r="C121">
+        <v>9.3500003218650818E-2</v>
+      </c>
+      <c r="D121">
+        <v>9.2799998819828033E-2</v>
+      </c>
+      <c r="E121">
+        <v>9.2399999499320984E-2</v>
+      </c>
+      <c r="F121">
+        <v>9.2399999499320984E-2</v>
+      </c>
+      <c r="G121">
+        <v>9.2699997127056122E-2</v>
+      </c>
+      <c r="H121">
+        <v>9.2699997127056122E-2</v>
+      </c>
+      <c r="I121">
+        <v>9.2399999499320984E-2</v>
+      </c>
+      <c r="J121">
+        <v>9.1700002551078796E-2</v>
+      </c>
+      <c r="K121">
+        <v>9.1899998486042023E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B122">
+        <v>0.12280000001192093</v>
+      </c>
+      <c r="C122">
+        <v>0.12319999933242798</v>
+      </c>
+      <c r="D122">
+        <v>0.12330000102519989</v>
+      </c>
+      <c r="E122">
+        <v>0.12290000170469284</v>
+      </c>
+      <c r="F122">
+        <v>0.12399999797344208</v>
+      </c>
+      <c r="G122">
+        <v>0.12300000339746475</v>
+      </c>
+      <c r="H122">
+        <v>0.12189999967813492</v>
+      </c>
+      <c r="I122">
+        <v>0.12349999696016312</v>
+      </c>
+      <c r="J122">
+        <v>0.12409999966621399</v>
+      </c>
+      <c r="K122">
+        <v>0.12080000340938568</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B123">
+        <v>9.08999964594841E-2</v>
+      </c>
+      <c r="C123">
+        <v>8.9699998497962952E-2</v>
+      </c>
+      <c r="D123">
+        <v>9.0499997138977051E-2</v>
+      </c>
+      <c r="E123">
+        <v>9.1200001537799835E-2</v>
+      </c>
+      <c r="F123">
+        <v>9.1099999845027924E-2</v>
+      </c>
+      <c r="G123">
+        <v>8.9299999177455902E-2</v>
+      </c>
+      <c r="H123">
+        <v>8.9100003242492676E-2</v>
+      </c>
+      <c r="I123">
+        <v>9.0099997818470001E-2</v>
+      </c>
+      <c r="J123">
+        <v>8.9900001883506775E-2</v>
+      </c>
+      <c r="K123">
+        <v>8.9699998497962952E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>55</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2438,7 +5754,7 @@
   <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>